<commit_message>
update Spain provinces data-charts and Euskadi hospitalized 2020.07.14
</commit_message>
<xml_diff>
--- a/data/original/spain/euskadi/datos-asistenciales.xlsx
+++ b/data/original/spain/euskadi/datos-asistenciales.xlsx
@@ -903,10 +903,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>385.0</v>
+        <v>386.0</v>
       </c>
       <c r="C14" t="n">
-        <v>155.0</v>
+        <v>156.0</v>
       </c>
       <c r="D14" t="n">
         <v>45.0</v>
@@ -970,10 +970,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>432.0</v>
+        <v>433.0</v>
       </c>
       <c r="C15" t="n">
-        <v>186.0</v>
+        <v>187.0</v>
       </c>
       <c r="D15" t="n">
         <v>49.0</v>
@@ -1037,10 +1037,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>462.0</v>
+        <v>463.0</v>
       </c>
       <c r="C16" t="n">
-        <v>197.0</v>
+        <v>198.0</v>
       </c>
       <c r="D16" t="n">
         <v>50.0</v>
@@ -3114,10 +3114,10 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1107.0</v>
+        <v>1109.0</v>
       </c>
       <c r="C47" t="n">
-        <v>161.0</v>
+        <v>163.0</v>
       </c>
       <c r="D47" t="n">
         <v>174.0</v>
@@ -3181,10 +3181,10 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>1036.0</v>
+        <v>1038.0</v>
       </c>
       <c r="C48" t="n">
-        <v>143.0</v>
+        <v>145.0</v>
       </c>
       <c r="D48" t="n">
         <v>149.0</v>
@@ -3248,10 +3248,10 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>964.0</v>
+        <v>966.0</v>
       </c>
       <c r="C49" t="n">
-        <v>131.0</v>
+        <v>133.0</v>
       </c>
       <c r="D49" t="n">
         <v>136.0</v>
@@ -3315,10 +3315,10 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>922.0</v>
+        <v>924.0</v>
       </c>
       <c r="C50" t="n">
-        <v>121.0</v>
+        <v>123.0</v>
       </c>
       <c r="D50" t="n">
         <v>126.0</v>
@@ -3382,10 +3382,10 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>841.0</v>
+        <v>843.0</v>
       </c>
       <c r="C51" t="n">
-        <v>110.0</v>
+        <v>112.0</v>
       </c>
       <c r="D51" t="n">
         <v>114.0</v>
@@ -3449,10 +3449,10 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>831.0</v>
+        <v>833.0</v>
       </c>
       <c r="C52" t="n">
-        <v>106.0</v>
+        <v>108.0</v>
       </c>
       <c r="D52" t="n">
         <v>118.0</v>
@@ -3516,10 +3516,10 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>831.0</v>
+        <v>833.0</v>
       </c>
       <c r="C53" t="n">
-        <v>108.0</v>
+        <v>110.0</v>
       </c>
       <c r="D53" t="n">
         <v>115.0</v>
@@ -8607,7 +8607,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>164.0</v>
+        <v>165.0</v>
       </c>
       <c r="C132" t="n">
         <v>26.0</v>
@@ -8619,7 +8619,7 @@
         <v>7.0</v>
       </c>
       <c r="F132" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="G132" t="n">
         <v>5.0</v>
@@ -8670,7 +8670,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>164.0</v>
+        <v>165.0</v>
       </c>
       <c r="C133" t="n">
         <v>28.0</v>
@@ -8682,7 +8682,7 @@
         <v>7.0</v>
       </c>
       <c r="F133" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="G133" t="n">
         <v>4.0</v>
@@ -8733,7 +8733,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>154.0</v>
+        <v>155.0</v>
       </c>
       <c r="C134" t="n">
         <v>24.0</v>
@@ -8745,7 +8745,7 @@
         <v>6.0</v>
       </c>
       <c r="F134" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="G134" t="n">
         <v>4.0</v>
@@ -8796,7 +8796,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>148.0</v>
+        <v>149.0</v>
       </c>
       <c r="C135" t="n">
         <v>25.0</v>
@@ -8808,7 +8808,7 @@
         <v>8.0</v>
       </c>
       <c r="F135" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="G135" t="n">
         <v>4.0</v>
@@ -9038,6 +9038,69 @@
         <v>5.0</v>
       </c>
       <c r="U138" t="n">
+        <v>34.0</v>
+      </c>
+    </row>
+    <row r="139" customHeight="true" ht="15.0">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>7/14/2020</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>164.0</v>
+      </c>
+      <c r="C139" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="D139" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="E139" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="F139" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="G139" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="H139"/>
+      <c r="I139" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="J139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K139" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="L139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M139" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="N139" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="O139" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="P139" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="Q139" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R139" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S139"/>
+      <c r="T139" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="U139" t="n">
         <v>34.0</v>
       </c>
     </row>
@@ -9888,10 +9951,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>64.0</v>
+        <v>65.0</v>
       </c>
       <c r="C14" t="n">
-        <v>34.0</v>
+        <v>35.0</v>
       </c>
       <c r="D14" t="n">
         <v>10.0</v>
@@ -12099,10 +12162,10 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>62.0</v>
+        <v>64.0</v>
       </c>
       <c r="C47" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="D47" t="n">
         <v>9.0</v>
@@ -17592,7 +17655,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="C132" t="n">
         <v>4.0</v>
@@ -17604,7 +17667,7 @@
         <v>4.0</v>
       </c>
       <c r="F132" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G132" t="n">
         <v>0.0</v>
@@ -18023,6 +18086,69 @@
         <v>1.0</v>
       </c>
       <c r="U138" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="139" customHeight="true" ht="15.0">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>7/14/2020</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C139" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D139" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="E139" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="F139" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G139" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H139"/>
+      <c r="I139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L139" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="M139" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="N139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S139"/>
+      <c r="T139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U139" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -19074,10 +19200,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
       <c r="C17" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="D17" t="n">
         <v>2.0</v>
@@ -21553,10 +21679,10 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>115.0</v>
+        <v>117.0</v>
       </c>
       <c r="C54" t="n">
-        <v>16.0</v>
+        <v>18.0</v>
       </c>
       <c r="D54" t="n">
         <v>26.0</v>
@@ -26829,7 +26955,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="C136" t="n">
         <v>3.0</v>
@@ -26841,7 +26967,7 @@
         <v>0.0</v>
       </c>
       <c r="F136" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G136" t="n">
         <v>0.0</v>
@@ -27008,6 +27134,69 @@
         <v>0.0</v>
       </c>
       <c r="U138" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="139" customHeight="true" ht="15.0">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>7/14/2020</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="C139" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D139" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="E139" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F139" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="G139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H139"/>
+      <c r="I139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J139" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L139" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S139"/>
+      <c r="T139" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="U139" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -32477,6 +32666,43 @@
       <c r="S138"/>
       <c r="T138"/>
       <c r="U138"/>
+    </row>
+    <row r="139" customHeight="true" ht="15.0">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>7/14/2020</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="C139" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D139" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="E139" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F139" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G139"/>
+      <c r="H139"/>
+      <c r="I139"/>
+      <c r="J139"/>
+      <c r="K139"/>
+      <c r="L139"/>
+      <c r="M139"/>
+      <c r="N139"/>
+      <c r="O139"/>
+      <c r="P139"/>
+      <c r="Q139"/>
+      <c r="R139"/>
+      <c r="S139"/>
+      <c r="T139"/>
+      <c r="U139"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -37948,6 +38174,43 @@
       <c r="T138"/>
       <c r="U138"/>
     </row>
+    <row r="139" customHeight="true" ht="15.0">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>7/14/2020</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G139"/>
+      <c r="H139"/>
+      <c r="I139"/>
+      <c r="J139"/>
+      <c r="K139"/>
+      <c r="L139"/>
+      <c r="M139"/>
+      <c r="N139"/>
+      <c r="O139"/>
+      <c r="P139"/>
+      <c r="Q139"/>
+      <c r="R139"/>
+      <c r="S139"/>
+      <c r="T139"/>
+      <c r="U139"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -43415,6 +43678,43 @@
       <c r="T138"/>
       <c r="U138"/>
     </row>
+    <row r="139" customHeight="true" ht="15.0">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>7/14/2020</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D139" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E139" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F139" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G139"/>
+      <c r="H139"/>
+      <c r="I139"/>
+      <c r="J139"/>
+      <c r="K139"/>
+      <c r="L139"/>
+      <c r="M139"/>
+      <c r="N139"/>
+      <c r="O139"/>
+      <c r="P139"/>
+      <c r="Q139"/>
+      <c r="R139"/>
+      <c r="S139"/>
+      <c r="T139"/>
+      <c r="U139"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -43616,7 +43916,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>982.0</v>
+        <v>984.0</v>
       </c>
       <c r="C4" t="n">
         <v>242.0</v>
@@ -43628,7 +43928,7 @@
         <v>61.0</v>
       </c>
       <c r="F4" t="n">
-        <v>110.0</v>
+        <v>111.0</v>
       </c>
       <c r="G4" t="n">
         <v>111.0</v>
@@ -43646,7 +43946,7 @@
         <v>15.0</v>
       </c>
       <c r="L4" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="M4" t="n">
         <v>9.0</v>
@@ -52285,7 +52585,7 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C137" t="n">
         <v>0.0</v>
@@ -52297,7 +52597,7 @@
         <v>0.0</v>
       </c>
       <c r="F137" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G137" t="n">
         <v>0.0</v>
@@ -52464,6 +52764,69 @@
         <v>0.0</v>
       </c>
       <c r="U139" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="140" customHeight="true" ht="15.0">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>7/14/2020</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H140"/>
+      <c r="I140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L140" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="M140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S140"/>
+      <c r="T140" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U140" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -57050,13 +57413,13 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="C79" t="n">
         <v>3.0</v>
       </c>
       <c r="D79" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E79" t="n">
         <v>0.0</v>
@@ -57168,7 +57531,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="C81" t="n">
         <v>0.0</v>
@@ -57211,7 +57574,7 @@
         <v>0.0</v>
       </c>
       <c r="Q81" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="R81"/>
       <c r="S81"/>
@@ -57685,7 +58048,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="C90" t="n">
         <v>0.0</v>
@@ -57694,7 +58057,7 @@
         <v>0.0</v>
       </c>
       <c r="E90" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F90" t="n">
         <v>1.0</v>
@@ -59346,13 +59709,13 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="C119" t="n">
         <v>0.0</v>
       </c>
       <c r="D119" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E119" t="n">
         <v>0.0</v>
@@ -59820,7 +60183,9 @@
         <v>0.0</v>
       </c>
       <c r="J127"/>
-      <c r="K127"/>
+      <c r="K127" t="n">
+        <v>0.0</v>
+      </c>
       <c r="L127" t="n">
         <v>1.0</v>
       </c>
@@ -59853,7 +60218,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="C128" t="n">
         <v>0.0</v>
@@ -59889,7 +60254,7 @@
         <v>0.0</v>
       </c>
       <c r="P128" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="Q128" t="n">
         <v>0.0</v>
@@ -59910,13 +60275,13 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C129" t="n">
         <v>1.0</v>
       </c>
       <c r="D129" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E129" t="n">
         <v>0.0</v>
@@ -59969,10 +60334,10 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C130" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D130" t="n">
         <v>0.0</v>
@@ -60026,19 +60391,19 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C131" t="n">
         <v>0.0</v>
       </c>
       <c r="D131" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E131" t="n">
         <v>1.0</v>
       </c>
       <c r="F131" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G131" t="n">
         <v>1.0</v>
@@ -60273,13 +60638,13 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C136" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D136" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E136" t="n">
         <v>1.0</v>
@@ -60306,8 +60671,51 @@
       <c r="Q136"/>
       <c r="R136"/>
       <c r="S136"/>
-      <c r="T136"/>
+      <c r="T136" t="n">
+        <v>0.0</v>
+      </c>
       <c r="U136"/>
+    </row>
+    <row r="137" customHeight="true" ht="15.0">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>7/14/2020</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C137" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D137" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E137" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F137" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G137" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H137"/>
+      <c r="I137"/>
+      <c r="J137"/>
+      <c r="K137"/>
+      <c r="L137"/>
+      <c r="M137"/>
+      <c r="N137"/>
+      <c r="O137"/>
+      <c r="P137" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Q137"/>
+      <c r="R137"/>
+      <c r="S137"/>
+      <c r="T137"/>
+      <c r="U137"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -65372,13 +65780,13 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C131" t="n">
         <v>0.0</v>
       </c>
       <c r="D131" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E131"/>
       <c r="F131"/>
@@ -65442,17 +65850,17 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="C133" t="n">
         <v>0.0</v>
       </c>
       <c r="D133" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E133"/>
       <c r="F133" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G133"/>
       <c r="H133"/>
@@ -65482,7 +65890,9 @@
       <c r="C134" t="n">
         <v>0.0</v>
       </c>
-      <c r="D134"/>
+      <c r="D134" t="n">
+        <v>0.0</v>
+      </c>
       <c r="E134"/>
       <c r="F134" t="n">
         <v>0.0</v>
@@ -65515,7 +65925,9 @@
       <c r="C135" t="n">
         <v>0.0</v>
       </c>
-      <c r="D135"/>
+      <c r="D135" t="n">
+        <v>0.0</v>
+      </c>
       <c r="E135"/>
       <c r="F135" t="n">
         <v>0.0</v>
@@ -65548,7 +65960,9 @@
       <c r="C136" t="n">
         <v>0.0</v>
       </c>
-      <c r="D136"/>
+      <c r="D136" t="n">
+        <v>0.0</v>
+      </c>
       <c r="E136"/>
       <c r="F136" t="n">
         <v>0.0</v>
@@ -65569,6 +65983,39 @@
       <c r="T136"/>
       <c r="U136"/>
     </row>
+    <row r="137" customHeight="true" ht="15.0">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>7/14/2020</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C137" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D137"/>
+      <c r="E137"/>
+      <c r="F137" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G137"/>
+      <c r="H137"/>
+      <c r="I137"/>
+      <c r="J137"/>
+      <c r="K137"/>
+      <c r="L137"/>
+      <c r="M137"/>
+      <c r="N137"/>
+      <c r="O137"/>
+      <c r="P137"/>
+      <c r="Q137"/>
+      <c r="R137"/>
+      <c r="S137"/>
+      <c r="T137"/>
+      <c r="U137"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>